<commit_message>
first idea for my project
</commit_message>
<xml_diff>
--- a/docs/exercise/GradedExercise.xlsx
+++ b/docs/exercise/GradedExercise.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samwurgler/switchdrive/_workfolder/webec/bewertete_uebung/docs/exercise/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16220" yWindow="28800" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="3440" yWindow="1440" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,11 @@
   <definedNames>
     <definedName name="TOTAL_POINTS">Sheet1!$I$32</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -119,7 +127,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> per Criteria</t>
@@ -143,7 +150,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> per Unit</t>
@@ -172,7 +178,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -255,12 +260,17 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -589,10 +599,10 @@
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
@@ -601,10 +611,10 @@
     <col min="6" max="6" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>23</v>
       </c>
@@ -627,7 +637,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D4">
         <v>5</v>
       </c>
@@ -638,7 +648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D5">
         <v>15</v>
       </c>
@@ -649,7 +659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -665,7 +675,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D8">
         <v>2</v>
       </c>
@@ -676,7 +686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D9">
         <v>2</v>
       </c>
@@ -687,7 +697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D10">
         <v>3</v>
       </c>
@@ -698,7 +708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D11">
         <v>5</v>
       </c>
@@ -709,7 +719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D12">
         <v>10</v>
       </c>
@@ -720,7 +730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
@@ -736,11 +746,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D15">
         <v>5</v>
       </c>
@@ -751,7 +761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D16">
         <v>5</v>
       </c>
@@ -762,7 +772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D17">
         <v>2</v>
       </c>
@@ -773,7 +783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D18">
         <v>2</v>
       </c>
@@ -784,7 +794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D19">
         <v>2</v>
       </c>
@@ -795,7 +805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D20">
         <v>2</v>
       </c>
@@ -806,7 +816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D21">
         <v>2</v>
       </c>
@@ -817,7 +827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
@@ -833,7 +843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D24">
         <v>5</v>
       </c>
@@ -844,7 +854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D25">
         <v>5</v>
       </c>
@@ -855,7 +865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D26">
         <v>5</v>
       </c>
@@ -866,7 +876,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D27">
         <v>5</v>
       </c>
@@ -877,7 +887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D28">
         <v>5</v>
       </c>
@@ -888,7 +898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
@@ -904,7 +914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
@@ -920,7 +930,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>30</v>
       </c>
@@ -937,10 +947,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>